<commit_message>
Added Validation for input
added validation for player ID and submit can now handle default values
</commit_message>
<xml_diff>
--- a/public/config.xlsx
+++ b/public/config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="66">
   <si>
     <t>Tab</t>
   </si>
@@ -99,12 +99,6 @@
   </si>
   <si>
     <t>multiline</t>
-  </si>
-  <si>
-    <t>Quantitative</t>
-  </si>
-  <si>
-    <t>Risk rank 1</t>
   </si>
   <si>
     <t>Yes, No</t>
@@ -210,6 +204,27 @@
   </si>
   <si>
     <t>Player's synergy as defined by the FIFA standards</t>
+  </si>
+  <si>
+    <t>Defence</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>Jorge</t>
+  </si>
+  <si>
+    <t>Team player with a very good physical strength, can support a false nine.</t>
+  </si>
+  <si>
+    <t>Please enter ID</t>
+  </si>
+  <si>
+    <t>Please enter Name</t>
+  </si>
+  <si>
+    <t>Defensive Midfield</t>
   </si>
 </sst>
 </file>
@@ -561,7 +576,7 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,16 +663,16 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
@@ -665,6 +680,9 @@
       <c r="F2" t="s">
         <v>23</v>
       </c>
+      <c r="I2" t="s">
+        <v>63</v>
+      </c>
       <c r="K2" t="s">
         <v>20</v>
       </c>
@@ -674,16 +692,16 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
@@ -691,6 +709,9 @@
       <c r="F3" t="s">
         <v>23</v>
       </c>
+      <c r="I3" t="s">
+        <v>64</v>
+      </c>
       <c r="K3" t="s">
         <v>20</v>
       </c>
@@ -700,16 +721,16 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
@@ -717,6 +738,9 @@
       <c r="F4" t="s">
         <v>23</v>
       </c>
+      <c r="I4" t="s">
+        <v>65</v>
+      </c>
       <c r="K4" t="s">
         <v>20</v>
       </c>
@@ -726,16 +750,16 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
@@ -744,10 +768,10 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I5" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="K5" t="s">
         <v>20</v>
@@ -758,16 +782,16 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -776,10 +800,10 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" t="s">
-        <v>26</v>
+        <v>56</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
       </c>
       <c r="K6" t="s">
         <v>20</v>
@@ -790,16 +814,16 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
@@ -808,7 +832,10 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="I7" t="s">
+        <v>60</v>
       </c>
       <c r="K7" t="s">
         <v>20</v>
@@ -819,19 +846,22 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
         <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="I8">
+        <v>25</v>
       </c>
       <c r="K8" t="s">
         <v>20</v>
@@ -842,16 +872,16 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
@@ -859,6 +889,9 @@
       <c r="F9" t="s">
         <v>23</v>
       </c>
+      <c r="I9" t="s">
+        <v>61</v>
+      </c>
       <c r="K9" t="s">
         <v>20</v>
       </c>
@@ -868,16 +901,16 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
         <v>22</v>
@@ -885,6 +918,9 @@
       <c r="F10" t="s">
         <v>24</v>
       </c>
+      <c r="I10" t="s">
+        <v>62</v>
+      </c>
       <c r="K10" t="s">
         <v>20</v>
       </c>
@@ -894,16 +930,16 @@
     </row>
     <row r="11" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
@@ -912,10 +948,10 @@
         <v>19</v>
       </c>
       <c r="G11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K11" t="s">
         <v>21</v>
@@ -924,7 +960,7 @@
         <v>24</v>
       </c>
       <c r="N11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="P11" t="s">
         <v>20</v>
@@ -932,16 +968,16 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -950,10 +986,10 @@
         <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K12" t="s">
         <v>21</v>
@@ -962,7 +998,7 @@
         <v>24</v>
       </c>
       <c r="N12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="P12" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Reading formula from config
Displaying dynamic content on the read-only input boxes based on the configuration file and the user inputs. yet to add in the calculation functionality.
</commit_message>
<xml_diff>
--- a/public/config.xlsx
+++ b/public/config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="83">
   <si>
     <t>Tab</t>
   </si>
@@ -225,6 +225,57 @@
   </si>
   <si>
     <t>Defensive Midfield</t>
+  </si>
+  <si>
+    <t>Player Stats</t>
+  </si>
+  <si>
+    <t>No. of clubs played for</t>
+  </si>
+  <si>
+    <t>Different clubs in Europe's top 5 leagues</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Goals scored for country</t>
+  </si>
+  <si>
+    <t>Goals scored for club</t>
+  </si>
+  <si>
+    <t>Goals scored in youth career</t>
+  </si>
+  <si>
+    <t>Goals scored by the player for the country</t>
+  </si>
+  <si>
+    <t>Goals scored by the player in their youth career</t>
+  </si>
+  <si>
+    <t>Goals scored by the player for all their clubs</t>
+  </si>
+  <si>
+    <t>Tab 3</t>
+  </si>
+  <si>
+    <t>Player Rating</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>read-only</t>
+  </si>
+  <si>
+    <t>Player club score</t>
+  </si>
+  <si>
+    <t>Comment on this</t>
+  </si>
+  <si>
+    <t>Player country score</t>
   </si>
 </sst>
 </file>
@@ -283,8 +334,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S12" totalsRowShown="0">
-  <autoFilter ref="A1:S12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S18" totalsRowShown="0">
+  <autoFilter ref="A1:S18"/>
   <tableColumns count="19">
     <tableColumn id="1" name="Tab"/>
     <tableColumn id="2" name="Section"/>
@@ -573,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,39 +979,39 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="165" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>51</v>
+        <v>67</v>
+      </c>
+      <c r="D11" t="s">
+        <v>68</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" t="s">
-        <v>26</v>
+        <v>54</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>81</v>
       </c>
       <c r="K11" t="s">
         <v>21</v>
       </c>
       <c r="L11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N11" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="P11" t="s">
         <v>20</v>
@@ -971,36 +1022,201 @@
         <v>29</v>
       </c>
       <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>20</v>
+      </c>
+      <c r="P12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>20</v>
+      </c>
+      <c r="P13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
+        <v>20</v>
+      </c>
+      <c r="P14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="165" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
         <v>49</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" t="s">
+        <v>24</v>
+      </c>
+      <c r="N17" t="s">
+        <v>27</v>
+      </c>
+      <c r="P17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
         <v>52</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D18" t="s">
         <v>53</v>
       </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
         <v>19</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G18" t="s">
         <v>25</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I18" t="s">
         <v>26</v>
       </c>
-      <c r="K12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="K18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" t="s">
         <v>24</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N18" t="s">
         <v>27</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P18" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added dynamic calculation logic
Was able to write custom functions to perform the calculations based on textual user inputs in the config file
</commit_message>
<xml_diff>
--- a/public/config.xlsx
+++ b/public/config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="93">
   <si>
     <t>Tab</t>
   </si>
@@ -275,7 +275,37 @@
     <t>Comment on this</t>
   </si>
   <si>
-    <t>Player country score</t>
+    <t>Is the player nice</t>
+  </si>
+  <si>
+    <t>Niceness scale of player</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has the player settled in life </t>
+  </si>
+  <si>
+    <t>Talk about player's personal life (marriage, kids)</t>
+  </si>
+  <si>
+    <t>Is the player around his prime</t>
+  </si>
+  <si>
+    <t>Near his prime in career in club and country football</t>
+  </si>
+  <si>
+    <t>should we buy the player</t>
+  </si>
+  <si>
+    <t>yesand(Does the player have good fan following, Is the player nice, Is the player around his prime)</t>
+  </si>
+  <si>
+    <t>Goals scored for country + Goals scored for club + Goals scored in youth career</t>
+  </si>
+  <si>
+    <t>Player goal score</t>
+  </si>
+  <si>
+    <t>Goals scored for club/No. of clubs played for</t>
   </si>
 </sst>
 </file>
@@ -334,8 +364,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S18" totalsRowShown="0">
-  <autoFilter ref="A1:S18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S22" totalsRowShown="0">
+  <autoFilter ref="A1:S22"/>
   <tableColumns count="19">
     <tableColumn id="1" name="Tab"/>
     <tableColumn id="2" name="Section"/>
@@ -624,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,7 +1142,7 @@
         <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="E15" t="s">
         <v>78</v>
@@ -1121,7 +1151,7 @@
         <v>79</v>
       </c>
       <c r="H15" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1141,7 +1171,7 @@
         <v>79</v>
       </c>
       <c r="H16" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="165" x14ac:dyDescent="0.25">
@@ -1218,6 +1248,122 @@
       </c>
       <c r="P18" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19" t="s">
+        <v>20</v>
+      </c>
+      <c r="P19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" t="s">
+        <v>20</v>
+      </c>
+      <c r="P20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" t="s">
+        <v>20</v>
+      </c>
+      <c r="P21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" t="s">
+        <v>79</v>
+      </c>
+      <c r="H22" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>